<commit_message>
Better exception handling for missing dates and fix input schedule for Leiding
</commit_message>
<xml_diff>
--- a/data/Leidingplanning 2017 date formatted zaterdag.xlsx
+++ b/data/Leidingplanning 2017 date formatted zaterdag.xlsx
@@ -1191,15 +1191,15 @@
   </sheetPr>
   <dimension ref="A1:CO65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CD1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CK1" activeCellId="0" sqref="CK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="90" min="3" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="90" min="3" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="91" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1207,268 +1207,268 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="n">
-        <v>43024.3958333333</v>
+        <v>43029.3958333333</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>43024.4027777778</v>
+        <v>43029.4027777778</v>
       </c>
       <c r="E1" s="2" t="n">
-        <v>43024.4097222222</v>
+        <v>43029.4097222222</v>
       </c>
       <c r="F1" s="2" t="n">
-        <v>43024.4166666667</v>
+        <v>43029.4166666667</v>
       </c>
       <c r="G1" s="2" t="n">
-        <v>43024.4236111111</v>
+        <v>43029.4236111111</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>43024.4305555556</v>
+        <v>43029.4305555556</v>
       </c>
       <c r="I1" s="2" t="n">
-        <v>43024.4375</v>
+        <v>43029.4375</v>
       </c>
       <c r="J1" s="2" t="n">
-        <v>43024.4444444445</v>
+        <v>43029.4444444445</v>
       </c>
       <c r="K1" s="2" t="n">
-        <v>43024.4513888889</v>
+        <v>43029.4513888889</v>
       </c>
       <c r="L1" s="2" t="n">
-        <v>43024.4583333333</v>
+        <v>43029.4583333333</v>
       </c>
       <c r="M1" s="2" t="n">
-        <v>43024.4652777778</v>
+        <v>43029.4652777778</v>
       </c>
       <c r="N1" s="2" t="n">
-        <v>43024.4722222222</v>
+        <v>43029.4722222222</v>
       </c>
       <c r="O1" s="2" t="n">
-        <v>43024.4791666667</v>
+        <v>43029.4791666667</v>
       </c>
       <c r="P1" s="2" t="n">
-        <v>43024.4861111111</v>
+        <v>43029.4861111111</v>
       </c>
       <c r="Q1" s="2" t="n">
-        <v>43024.4930555556</v>
+        <v>43029.4930555556</v>
       </c>
       <c r="R1" s="2" t="n">
-        <v>43024.5</v>
+        <v>43029.5</v>
       </c>
       <c r="S1" s="2" t="n">
-        <v>43024.5069444445</v>
+        <v>43029.5069444445</v>
       </c>
       <c r="T1" s="2" t="n">
-        <v>43024.5138888889</v>
+        <v>43029.5138888889</v>
       </c>
       <c r="U1" s="2" t="n">
-        <v>43024.5208333333</v>
+        <v>43029.5208333333</v>
       </c>
       <c r="V1" s="2" t="n">
-        <v>43024.5277777778</v>
+        <v>43029.5277777778</v>
       </c>
       <c r="W1" s="2" t="n">
-        <v>43024.5347222222</v>
+        <v>43029.5347222222</v>
       </c>
       <c r="X1" s="2" t="n">
-        <v>43024.5416666667</v>
+        <v>43029.5416666667</v>
       </c>
       <c r="Y1" s="2" t="n">
-        <v>43024.5486111111</v>
+        <v>43029.5486111111</v>
       </c>
       <c r="Z1" s="2" t="n">
-        <v>43024.5555555556</v>
+        <v>43029.5555555556</v>
       </c>
       <c r="AA1" s="2" t="n">
-        <v>43024.5625</v>
+        <v>43029.5625</v>
       </c>
       <c r="AB1" s="2" t="n">
-        <v>43024.5694444445</v>
+        <v>43029.5694444445</v>
       </c>
       <c r="AC1" s="2" t="n">
-        <v>43024.5763888889</v>
+        <v>43029.5763888889</v>
       </c>
       <c r="AD1" s="2" t="n">
-        <v>43024.5833333334</v>
+        <v>43029.5833333334</v>
       </c>
       <c r="AE1" s="2" t="n">
-        <v>43024.5902777778</v>
+        <v>43029.5902777778</v>
       </c>
       <c r="AF1" s="2" t="n">
-        <v>43024.5972222222</v>
+        <v>43029.5972222222</v>
       </c>
       <c r="AG1" s="2" t="n">
-        <v>43024.6041666667</v>
+        <v>43029.6041666667</v>
       </c>
       <c r="AH1" s="2" t="n">
-        <v>43024.6111111111</v>
+        <v>43029.6111111111</v>
       </c>
       <c r="AI1" s="2" t="n">
-        <v>43024.6180555556</v>
+        <v>43029.6180555556</v>
       </c>
       <c r="AJ1" s="2" t="n">
-        <v>43024.625</v>
+        <v>43029.625</v>
       </c>
       <c r="AK1" s="2" t="n">
-        <v>43024.6319444445</v>
+        <v>43029.6319444445</v>
       </c>
       <c r="AL1" s="2" t="n">
-        <v>43024.6388888889</v>
+        <v>43029.6388888889</v>
       </c>
       <c r="AM1" s="2" t="n">
-        <v>43024.6458333334</v>
+        <v>43029.6458333334</v>
       </c>
       <c r="AN1" s="2" t="n">
-        <v>43024.6527777778</v>
+        <v>43029.6527777778</v>
       </c>
       <c r="AO1" s="2" t="n">
-        <v>43024.6597222223</v>
+        <v>43029.6597222223</v>
       </c>
       <c r="AP1" s="2" t="n">
-        <v>43024.6666666667</v>
+        <v>43029.6666666667</v>
       </c>
       <c r="AQ1" s="2" t="n">
-        <v>43024.6736111111</v>
+        <v>43029.6736111111</v>
       </c>
       <c r="AR1" s="2" t="n">
-        <v>43024.6805555556</v>
+        <v>43029.6805555556</v>
       </c>
       <c r="AS1" s="2" t="n">
-        <v>43024.6875</v>
+        <v>43029.6875</v>
       </c>
       <c r="AT1" s="2" t="n">
-        <v>43024.6944444445</v>
+        <v>43029.6944444445</v>
       </c>
       <c r="AU1" s="2" t="n">
-        <v>43024.7013888889</v>
+        <v>43029.7013888889</v>
       </c>
       <c r="AV1" s="2" t="n">
-        <v>43024.7083333334</v>
+        <v>43029.7083333334</v>
       </c>
       <c r="AW1" s="2" t="n">
-        <v>43024.7152777778</v>
+        <v>43029.7152777778</v>
       </c>
       <c r="AX1" s="2" t="n">
-        <v>43024.7222222222</v>
+        <v>43029.7222222223</v>
       </c>
       <c r="AY1" s="2" t="n">
-        <v>43024.7291666667</v>
+        <v>43029.7291666667</v>
       </c>
       <c r="AZ1" s="2" t="n">
-        <v>43024.7361111111</v>
+        <v>43029.7361111111</v>
       </c>
       <c r="BA1" s="2" t="n">
-        <v>43024.7430555556</v>
+        <v>43029.7430555556</v>
       </c>
       <c r="BB1" s="2" t="n">
-        <v>43024.75</v>
+        <v>43029.75</v>
       </c>
       <c r="BC1" s="2" t="n">
-        <v>43024.7569444445</v>
+        <v>43029.7569444445</v>
       </c>
       <c r="BD1" s="2" t="n">
-        <v>43024.7638888889</v>
+        <v>43029.7638888889</v>
       </c>
       <c r="BE1" s="2" t="n">
-        <v>43024.7708333334</v>
+        <v>43029.7708333334</v>
       </c>
       <c r="BF1" s="2" t="n">
-        <v>43024.7777777778</v>
+        <v>43029.7777777778</v>
       </c>
       <c r="BG1" s="2" t="n">
-        <v>43024.7847222223</v>
+        <v>43029.7847222223</v>
       </c>
       <c r="BH1" s="2" t="n">
-        <v>43024.7916666667</v>
+        <v>43029.7916666667</v>
       </c>
       <c r="BI1" s="2" t="n">
-        <v>43024.7986111112</v>
+        <v>43029.7986111111</v>
       </c>
       <c r="BJ1" s="2" t="n">
-        <v>43024.8055555556</v>
+        <v>43029.8055555556</v>
       </c>
       <c r="BK1" s="2" t="n">
-        <v>43024.8125</v>
+        <v>43029.8125</v>
       </c>
       <c r="BL1" s="2" t="n">
-        <v>43024.8194444445</v>
+        <v>43029.8194444445</v>
       </c>
       <c r="BM1" s="2" t="n">
-        <v>43024.8263888889</v>
+        <v>43029.8263888889</v>
       </c>
       <c r="BN1" s="2" t="n">
-        <v>43024.8333333334</v>
+        <v>43029.8333333334</v>
       </c>
       <c r="BO1" s="2" t="n">
-        <v>43024.8402777778</v>
+        <v>43029.8402777778</v>
       </c>
       <c r="BP1" s="2" t="n">
-        <v>43024.8472222223</v>
+        <v>43029.8472222223</v>
       </c>
       <c r="BQ1" s="2" t="n">
-        <v>43024.8541666667</v>
+        <v>43029.8541666667</v>
       </c>
       <c r="BR1" s="2" t="n">
-        <v>43024.8611111112</v>
+        <v>43029.8611111112</v>
       </c>
       <c r="BS1" s="2" t="n">
-        <v>43024.8680555556</v>
+        <v>43029.8680555556</v>
       </c>
       <c r="BT1" s="2" t="n">
-        <v>43024.875</v>
+        <v>43029.875</v>
       </c>
       <c r="BU1" s="2" t="n">
-        <v>43024.8819444445</v>
+        <v>43029.8819444445</v>
       </c>
       <c r="BV1" s="2" t="n">
-        <v>43024.8888888889</v>
+        <v>43029.8888888889</v>
       </c>
       <c r="BW1" s="2" t="n">
-        <v>43024.8958333334</v>
+        <v>43029.8958333334</v>
       </c>
       <c r="BX1" s="2" t="n">
-        <v>43024.9027777778</v>
+        <v>43029.9027777778</v>
       </c>
       <c r="BY1" s="2" t="n">
-        <v>43024.9097222223</v>
+        <v>43029.9097222223</v>
       </c>
       <c r="BZ1" s="2" t="n">
-        <v>43024.9166666667</v>
+        <v>43029.9166666667</v>
       </c>
       <c r="CA1" s="2" t="n">
-        <v>43024.9236111112</v>
+        <v>43029.9236111112</v>
       </c>
       <c r="CB1" s="2" t="n">
-        <v>43024.9305555556</v>
+        <v>43029.9305555556</v>
       </c>
       <c r="CC1" s="2" t="n">
-        <v>43024.9375</v>
+        <v>43029.9375</v>
       </c>
       <c r="CD1" s="2" t="n">
-        <v>43024.9444444445</v>
+        <v>43029.9444444445</v>
       </c>
       <c r="CE1" s="2" t="n">
-        <v>43024.9513888889</v>
+        <v>43029.9513888889</v>
       </c>
       <c r="CF1" s="2" t="n">
-        <v>43024.9583333334</v>
+        <v>43029.9583333334</v>
       </c>
       <c r="CG1" s="2" t="n">
-        <v>43024.9652777778</v>
+        <v>43029.9652777778</v>
       </c>
       <c r="CH1" s="2" t="n">
-        <v>43024.9722222223</v>
+        <v>43029.9722222223</v>
       </c>
       <c r="CI1" s="2" t="n">
-        <v>43024.9791666667</v>
+        <v>43029.9791666667</v>
       </c>
       <c r="CJ1" s="2" t="n">
-        <v>43024.9861111112</v>
+        <v>43029.9861111112</v>
       </c>
       <c r="CK1" s="2" t="n">
-        <v>43024.9930555556</v>
+        <v>43029.9930555556</v>
       </c>
       <c r="CL1" s="2" t="n">
-        <v>43025</v>
+        <v>43030.0000000001</v>
       </c>
       <c r="CM1" s="3"/>
       <c r="CN1" s="4"/>

</xml_diff>